<commit_message>
fix pubmed nipah bug file
</commit_message>
<xml_diff>
--- a/Pubmed/Nipah/ReferenceSummary_Genbank_Jan13.xlsx
+++ b/Pubmed/Nipah/ReferenceSummary_Genbank_Jan13.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaimingtao/HIVDB/GenBankRefs/Pubmed/Nipah/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FFD60B0-D681-FC4E-BE50-AD4FD9FDA071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B607F1DB-2E80-414A-AF94-E251316C7183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="640" yWindow="500" windowWidth="37760" windowHeight="21100" xr2:uid="{3031CDAD-EDE9-504F-A9EA-0D1529922A9B}"/>
   </bookViews>
@@ -161,9 +161,6 @@
     <t>cerebrospinal fluid, human brain tissue, porcine lung tissue, canine brain tissue, and feline brain tissue</t>
   </si>
   <si>
-    <t>at</t>
-  </si>
-  <si>
     <t>Bangladesh</t>
   </si>
   <si>
@@ -174,6 +171,9 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Bat</t>
   </si>
 </sst>
 </file>
@@ -644,7 +644,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -803,25 +803,25 @@
         <v>32</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P3" s="1">
         <v>2010</v>
       </c>
       <c r="Q3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>37</v>
       </c>
       <c r="U3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V3" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>